<commit_message>
chore: contamination, delete segmented models, replace by spearman's tests => OC pesticides
</commit_message>
<xml_diff>
--- a/inst/results/data_contam/OC_pesticides/summarised_levels_data_OC_pesticides_ww.xlsx
+++ b/inst/results/data_contam/OC_pesticides/summarised_levels_data_OC_pesticides_ww.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -351,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,54 +361,102 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ESTUARY</t>
+          <t>PARAMETRE_LIBELLE</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>PARAMETRE_LIBELLE</t>
+          <t>First 5 years</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>median_ng_gww</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>median_1</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>median_2</t>
+          <t>Last 5 years</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Gironde</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
           <t>Gamma-HCH</t>
         </is>
+      </c>
+      <c r="B2">
+        <v>1.3865</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>336</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>sum_DDT</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>15.63015</v>
+      </c>
+      <c r="C3">
+        <v>1.112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ESTUARY</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PARAMETRE_LIBELLE</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>First 5 years</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Last 5 years</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Gironde</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Gamma-HCH</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>0.9743000000000001</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>Loire</t>
         </is>
       </c>
@@ -417,12 +466,9 @@
         </is>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1.3579</v>
       </c>
       <c r="D3">
-        <v>468.2</v>
-      </c>
-      <c r="E3">
         <v>0</v>
       </c>
     </row>
@@ -438,12 +484,9 @@
         </is>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>2.2463</v>
       </c>
       <c r="D4">
-        <v>774.6</v>
-      </c>
-      <c r="E4">
         <v>0</v>
       </c>
     </row>
@@ -459,13 +502,10 @@
         </is>
       </c>
       <c r="C5">
+        <v>15.77605</v>
+      </c>
+      <c r="D5">
         <v>1.737</v>
-      </c>
-      <c r="D5">
-        <v>1.231</v>
-      </c>
-      <c r="E5">
-        <v>0.1355</v>
       </c>
     </row>
     <row r="6">
@@ -480,13 +520,10 @@
         </is>
       </c>
       <c r="C6">
+        <v>12.28675</v>
+      </c>
+      <c r="D6">
         <v>0.5519000000000001</v>
-      </c>
-      <c r="D6">
-        <v>0.9584</v>
-      </c>
-      <c r="E6">
-        <v>0.04305</v>
       </c>
     </row>
     <row r="7">
@@ -501,13 +538,10 @@
         </is>
       </c>
       <c r="C7">
+        <v>23.24085</v>
+      </c>
+      <c r="D7">
         <v>1.7117</v>
-      </c>
-      <c r="D7">
-        <v>1.813</v>
-      </c>
-      <c r="E7">
-        <v>0.1335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>